<commit_message>
feat: add data cleaning, analysis, and visual reports for dataset 105
</commit_message>
<xml_diff>
--- a/laporan_ringkasan_akses.xlsx
+++ b/laporan_ringkasan_akses.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t>Total Log</t>
   </si>
@@ -39,30 +39,36 @@
     <t>count</t>
   </si>
   <si>
-    <t>Anggi Mahendra Dirga</t>
-  </si>
-  <si>
-    <t>Affandi</t>
-  </si>
-  <si>
-    <t>Meysa Dwi Pangesti</t>
-  </si>
-  <si>
-    <t>Restu Abdul Nova</t>
+    <t>Ahmad Nur Hidayat</t>
   </si>
   <si>
     <t>Master</t>
   </si>
   <si>
-    <t>Norma Butar Butar</t>
-  </si>
-  <si>
-    <t>V</t>
+    <t>Ingrid Vera Mour</t>
+  </si>
+  <si>
+    <t>Nafis</t>
+  </si>
+  <si>
+    <t>Housekeeping</t>
   </si>
   <si>
     <t>Shift Midle</t>
   </si>
   <si>
+    <t>Triswantoro</t>
+  </si>
+  <si>
+    <t>Metia Shanti Wulanda</t>
+  </si>
+  <si>
+    <t>Orbani</t>
+  </si>
+  <si>
+    <t>Lucky Hendrawan</t>
+  </si>
+  <si>
     <t>card_no.</t>
   </si>
   <si>
@@ -75,15 +81,15 @@
     <t>Jumlah Penggunaan</t>
   </si>
   <si>
+    <t>Master Card</t>
+  </si>
+  <si>
+    <t>HSKP Card</t>
+  </si>
+  <si>
     <t>Guest Card</t>
   </si>
   <si>
-    <t>Master Card</t>
-  </si>
-  <si>
-    <t>HSKP Card</t>
-  </si>
-  <si>
     <t>event_ord.</t>
   </si>
   <si>
@@ -117,43 +123,46 @@
     <t>waktu_singkat</t>
   </si>
   <si>
+    <t>front office</t>
+  </si>
+  <si>
     <t>vino</t>
   </si>
   <si>
-    <t>vani</t>
-  </si>
-  <si>
-    <t>18/06/2025 05:09:35</t>
-  </si>
-  <si>
-    <t>16/06/2025 23:11:32</t>
-  </si>
-  <si>
-    <t>15/06/2025 18:49:32</t>
-  </si>
-  <si>
-    <t>14/06/2025 20:30:07</t>
-  </si>
-  <si>
-    <t>2025-06-18 05:07:00</t>
-  </si>
-  <si>
-    <t>2025-06-18 05:00:00</t>
-  </si>
-  <si>
-    <t>2025-06-17 05:43:00</t>
-  </si>
-  <si>
-    <t>2025-06-17 05:14:00</t>
-  </si>
-  <si>
-    <t>2025-06-16 05:57:00</t>
-  </si>
-  <si>
-    <t>2025-06-15 00:24:00</t>
-  </si>
-  <si>
-    <t>2025-06-15 00:05:00</t>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>eko</t>
+  </si>
+  <si>
+    <t>18/06/2025 05:40:40</t>
+  </si>
+  <si>
+    <t>07/01/2023 22:19:13</t>
+  </si>
+  <si>
+    <t>09/06/2025 04:26:48</t>
+  </si>
+  <si>
+    <t>07/01/2025 06:33:52</t>
+  </si>
+  <si>
+    <t>2025-06-18 05:47:00</t>
+  </si>
+  <si>
+    <t>2025-06-18 05:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-18 05:34:00</t>
+  </si>
+  <si>
+    <t>2025-06-17 03:32:00</t>
+  </si>
+  <si>
+    <t>2025-06-12 05:26:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 04:23:00</t>
   </si>
 </sst>
 </file>
@@ -539,16 +548,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -558,7 +567,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -574,26 +583,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -622,15 +631,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -638,15 +647,15 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -654,7 +663,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -662,34 +671,58 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -699,7 +732,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -715,15 +748,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>45822</v>
+        <v>45815</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>45823</v>
+        <v>45816</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -731,34 +764,74 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>45824</v>
+        <v>45817</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>45825</v>
+        <v>45819</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>45826</v>
+        <v>45820</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
+        <v>45821</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2">
+        <v>45822</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2">
+        <v>45823</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2">
+        <v>45825</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2">
+        <v>45826</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2">
         <v>45827</v>
       </c>
-      <c r="B7">
-        <v>3</v>
+      <c r="B12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -768,7 +841,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -787,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -795,7 +868,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -803,7 +876,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -811,7 +884,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -819,7 +892,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -827,7 +900,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -835,7 +908,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -843,6 +916,22 @@
         <v>13</v>
       </c>
       <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
     </row>
@@ -853,7 +942,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -861,86 +950,86 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>13422</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>13390</v>
+        <v>10875</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>13406</v>
+        <v>13313</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>13377</v>
+        <v>13274</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>60</v>
+        <v>13423</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -948,40 +1037,68 @@
         <v>7516</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>13414</v>
+        <v>13386</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>13441</v>
+        <v>13344</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>13333</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>13429</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
         <v>1</v>
       </c>
     </row>
@@ -992,7 +1109,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1000,69 +1117,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3">
-        <v>45826.21319444444</v>
+        <v>45826.24097222222</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2">
-        <v>13422</v>
+        <v>13423</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L2" s="2">
         <v>45826</v>
@@ -1071,30 +1188,30 @@
         <v>5</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="B3" s="3">
-        <v>45826.20833333334</v>
+        <v>45826.23611111111</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3">
-        <v>13422</v>
+        <v>13423</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L3" s="2">
         <v>45826</v>
@@ -1103,167 +1220,153 @@
         <v>5</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>178</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3">
-        <v>45825.23819444444</v>
+        <v>45826.23194444444</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E4">
-        <v>13406</v>
+        <v>13423</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L4" s="2">
-        <v>45825</v>
+        <v>45826</v>
       </c>
       <c r="M4">
         <v>5</v>
       </c>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B5" s="3">
-        <v>45825.21805555555</v>
+        <v>45825.14722222222</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>13406</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
       </c>
       <c r="L5" s="2">
         <v>45825</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>257</v>
+        <v>313</v>
       </c>
       <c r="B6" s="3">
-        <v>45824.24791666667</v>
+        <v>45820.22638888889</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6">
-        <v>13390</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
         <v>36</v>
       </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
       <c r="L6" s="2">
-        <v>45824</v>
+        <v>45820</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
-        <v>359</v>
+        <v>391</v>
       </c>
       <c r="B7" s="3">
-        <v>45823.01666666667</v>
+        <v>45817.18263888889</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E7">
-        <v>13377</v>
+        <v>13313</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L7" s="2">
-        <v>45823</v>
+        <v>45817</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8">
-        <v>375</v>
-      </c>
-      <c r="B8" s="3">
-        <v>45823.00347222222</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8">
-        <v>13377</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="2">
-        <v>45823</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>